<commit_message>
progress for fall rec/2025
</commit_message>
<xml_diff>
--- a/src/data/current_data/directors_currentdata.xlsx
+++ b/src/data/current_data/directors_currentdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -19,80 +19,62 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Malak Shahin</t>
+    <t>Neeva Mehta</t>
   </si>
   <si>
     <t xml:space="preserve">Marketing
 </t>
   </si>
   <si>
-    <t>Tirza Kunaidy</t>
+    <t>Emily Guo</t>
   </si>
   <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Jessica Kwan</t>
+    <t>Vansh Mehta</t>
   </si>
   <si>
     <t>Professional Development</t>
   </si>
   <si>
-    <t>Shreya Jagannathan</t>
-  </si>
-  <si>
-    <t>Tiffany Zhang</t>
+    <t>Leo Alejandro Munoz</t>
   </si>
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Lauren Nguyen</t>
+    <t>Asmitha Chunchu</t>
   </si>
   <si>
-    <t>Mia Ness</t>
+    <t>Lohit Potnuru</t>
   </si>
   <si>
     <t>Brotherhood and Social Activities</t>
   </si>
   <si>
-    <t>Vanessa Chok</t>
+    <t>Sanika Patwardhan</t>
   </si>
   <si>
-    <t>James Kent</t>
-  </si>
-  <si>
-    <t>Investment</t>
-  </si>
-  <si>
-    <t>Brendon Sato</t>
-  </si>
-  <si>
-    <t>Joy Bae</t>
+    <t>Siena Dunn</t>
   </si>
   <si>
     <t>Content Creation</t>
   </si>
   <si>
-    <t>Ryan Chung</t>
+    <t>Aditya Aggarwal</t>
   </si>
   <si>
     <t>Fundraising</t>
   </si>
   <si>
-    <t>Isaac Martinez</t>
-  </si>
-  <si>
-    <t>Riya Kapadekar</t>
+    <t>Aaron Park</t>
   </si>
   <si>
     <t>External Relations</t>
   </si>
   <si>
-    <t>Joseph Whittaker</t>
-  </si>
-  <si>
-    <t>Mirsab Mirza</t>
+    <t>TBA</t>
   </si>
   <si>
     <t>Strategic Development</t>
@@ -102,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -130,11 +112,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -169,9 +146,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +388,7 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="21.0" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -431,134 +405,114 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" ht="20.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="3" t="s">
+    <row r="11">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -5437,31 +5391,6 @@
       <c r="A995" s="4"/>
       <c r="B995" s="4"/>
       <c r="C995" s="4"/>
-    </row>
-    <row r="996" ht="15.75" customHeight="1">
-      <c r="A996" s="4"/>
-      <c r="B996" s="4"/>
-      <c r="C996" s="4"/>
-    </row>
-    <row r="997" ht="15.75" customHeight="1">
-      <c r="A997" s="4"/>
-      <c r="B997" s="4"/>
-      <c r="C997" s="4"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="A998" s="4"/>
-      <c r="B998" s="4"/>
-      <c r="C998" s="4"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="A999" s="4"/>
-      <c r="B999" s="4"/>
-      <c r="C999" s="4"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="4"/>
-      <c r="C1000" s="4"/>
     </row>
   </sheetData>
   <printOptions/>

</xml_diff>